<commit_message>
event storming de reservas finalizado y ajustes en otro
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Event Storming/Agendas - Event Storming.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Event Storming/Agendas - Event Storming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Event Storming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C28265-0FA3-47AB-A0EE-9977A5CA0D50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB47941C-CABF-4999-9E83-FC3FDABD2089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{FFDB2CDE-A71C-41B2-9368-C2C506410E3B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FFDB2CDE-A71C-41B2-9368-C2C506410E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="1" r:id="rId1"/>
@@ -984,6 +984,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1008,132 +1026,198 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1142,90 +1226,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1641,7 +1641,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1652,39 +1652,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA54A37-9234-4843-BCF9-75FA1FE96664}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="31"/>
-    </row>
-    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="36"/>
+      <c r="D1" s="37"/>
+    </row>
+    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1708,12 +1708,12 @@
       <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="27" t="str">
+      <c r="D4" s="33" t="str">
         <f>$B$1</f>
         <v>Agendas</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1723,9 +1723,9 @@
       <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="28"/>
-    </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="D5" s="34"/>
+    </row>
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1735,7 +1735,7 @@
       <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="29"/>
+      <c r="D6" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1760,108 +1760,108 @@
       <selection activeCell="F15" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="29.85546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="9" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="29.88671875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="9" customWidth="1"/>
     <col min="8" max="8" width="31" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="37.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="9" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="9"/>
+    <col min="13" max="13" width="46.33203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="61"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
+      <c r="L2" s="47"/>
+      <c r="M2" s="48"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="62" t="str">
+      <c r="B3" s="49" t="str">
         <f>'Listado Objetos Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada una de las zonas comúnes que tendrán una agenda y respectivos turnos.</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="64"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
+      <c r="K3" s="50"/>
+      <c r="L3" s="50"/>
+      <c r="M3" s="51"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="66"/>
+      <c r="C4" s="53"/>
       <c r="D4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="67" t="s">
+      <c r="F4" s="55"/>
+      <c r="G4" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="68"/>
+      <c r="H4" s="57"/>
       <c r="I4" s="16" t="s">
         <v>26</v>
       </c>
@@ -1871,52 +1871,52 @@
       <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="69" t="s">
+      <c r="L4" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="72" t="s">
+      <c r="M4" s="61" t="s">
         <v>30</v>
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="52" t="s">
+      <c r="F5" s="55"/>
+      <c r="G5" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="73"/>
+      <c r="I5" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="56" t="s">
+      <c r="J5" s="76" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="68" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="70"/>
-      <c r="M5" s="73"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="76"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="49"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="62"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="65"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
@@ -1929,276 +1929,303 @@
       <c r="H6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="71"/>
-      <c r="M6" s="74"/>
-    </row>
-    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A7" s="97" t="s">
+      <c r="I6" s="75"/>
+      <c r="J6" s="77"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="60"/>
+      <c r="M6" s="63"/>
+    </row>
+    <row r="7" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="81" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="78" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="78" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="94" t="s">
+      <c r="D7" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="78" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="98" t="s">
+      <c r="H7" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94" t="s">
+      <c r="I7" s="78"/>
+      <c r="J7" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94" t="s">
+      <c r="K7" s="78"/>
+      <c r="L7" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="M7" s="99" t="s">
+      <c r="M7" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="100"/>
-      <c r="B8" s="95"/>
-      <c r="C8" s="95"/>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-      <c r="F8" s="95"/>
-      <c r="G8" s="94" t="s">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="82"/>
+      <c r="B8" s="79"/>
+      <c r="C8" s="79"/>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
+      <c r="F8" s="79"/>
+      <c r="G8" s="78" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="94" t="s">
+      <c r="H8" s="78" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="95"/>
-      <c r="J8" s="95"/>
-      <c r="K8" s="95"/>
-      <c r="L8" s="95"/>
-      <c r="M8" s="101" t="s">
+      <c r="I8" s="79"/>
+      <c r="J8" s="79"/>
+      <c r="K8" s="79"/>
+      <c r="L8" s="79"/>
+      <c r="M8" s="41" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="100"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="102"/>
-    </row>
-    <row r="10" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="103"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
-      <c r="I10" s="96"/>
-      <c r="J10" s="96"/>
-      <c r="K10" s="96"/>
-      <c r="L10" s="96"/>
-      <c r="M10" s="104" t="s">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="82"/>
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="79"/>
+      <c r="H9" s="79"/>
+      <c r="I9" s="79"/>
+      <c r="J9" s="79"/>
+      <c r="K9" s="79"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="42"/>
+    </row>
+    <row r="10" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="83"/>
+      <c r="B10" s="80"/>
+      <c r="C10" s="80"/>
+      <c r="D10" s="80"/>
+      <c r="E10" s="80"/>
+      <c r="F10" s="80"/>
+      <c r="G10" s="80"/>
+      <c r="H10" s="80"/>
+      <c r="I10" s="80"/>
+      <c r="J10" s="80"/>
+      <c r="K10" s="80"/>
+      <c r="L10" s="80"/>
+      <c r="M10" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="36" t="s">
+      <c r="F11" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36" t="s">
+      <c r="I11" s="43"/>
+      <c r="J11" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="36"/>
-      <c r="L11" s="36" t="s">
+      <c r="K11" s="43"/>
+      <c r="L11" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="M11" s="99" t="s">
+      <c r="M11" s="28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
-      <c r="L12" s="37"/>
-      <c r="M12" s="105" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="44"/>
+      <c r="M12" s="30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="84" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="94" t="s">
+      <c r="G13" s="78" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="94" t="s">
+      <c r="H13" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36" t="s">
+      <c r="I13" s="43"/>
+      <c r="J13" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="36"/>
-      <c r="L13" s="36" t="s">
+      <c r="K13" s="43"/>
+      <c r="L13" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="36" t="s">
+      <c r="M13" s="43" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
-      <c r="M14" s="37"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
+    <row r="14" spans="1:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="85"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
+      <c r="M14" s="44"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="86" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="35" t="s">
+      <c r="D15" s="86" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="86" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="94" t="s">
+      <c r="G15" s="78" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="94" t="s">
+      <c r="H15" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35" t="s">
+      <c r="I15" s="86"/>
+      <c r="J15" s="86" t="s">
         <v>46</v>
       </c>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35" t="s">
+      <c r="K15" s="86"/>
+      <c r="L15" s="86" t="s">
         <v>45</v>
       </c>
-      <c r="M15" s="35" t="s">
+      <c r="M15" s="86" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="96"/>
-      <c r="H16" s="96"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
+    <row r="16" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="86"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="80"/>
+      <c r="H16" s="80"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="I7:I10"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2215,45 +2242,18 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{887014DF-6A3A-42A6-91E6-4E5CFF547499}"/>
@@ -2271,108 +2271,108 @@
       <selection activeCell="H7" sqref="H7:H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="9" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="9" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="9" customWidth="1"/>
     <col min="8" max="8" width="28" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="9" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="9"/>
+    <col min="13" max="13" width="46.33203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="86" t="str">
+      <c r="B2" s="87" t="str">
         <f>'Listado Objetos Dominio'!A5</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="88"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos Dominio'!B5</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="81"/>
+      <c r="C4" s="91"/>
       <c r="D4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="82"/>
-      <c r="G4" s="90" t="s">
+      <c r="F4" s="92"/>
+      <c r="G4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="90"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="16" t="s">
         <v>26</v>
       </c>
@@ -2382,52 +2382,52 @@
       <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="91" t="s">
+      <c r="L4" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="92" t="s">
+      <c r="M4" s="95" t="s">
         <v>30</v>
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="93" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="96" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="83" t="s">
+      <c r="F5" s="92"/>
+      <c r="G5" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84" t="s">
+      <c r="H5" s="100"/>
+      <c r="I5" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="85" t="s">
+      <c r="J5" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="80" t="s">
+      <c r="K5" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="92"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="49"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="95"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="96"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
@@ -2440,83 +2440,83 @@
       <c r="H6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="92"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
+      <c r="I6" s="101"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="95"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="36" t="s">
+      <c r="D7" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="36" t="s">
+      <c r="G7" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36" t="s">
+      <c r="I7" s="43"/>
+      <c r="J7" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36" t="s">
+      <c r="K7" s="43"/>
+      <c r="L7" s="43" t="s">
         <v>74</v>
       </c>
       <c r="M7" s="25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="45"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="37"/>
-      <c r="F8" s="37"/>
-      <c r="G8" s="37"/>
-      <c r="H8" s="37"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="37"/>
-      <c r="L8" s="37"/>
+    <row r="8" spans="1:14" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="99"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
       <c r="M8" s="25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+    <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="98" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="36" t="s">
+      <c r="D9" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="36" t="s">
+      <c r="F9" s="43" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="21" t="s">
@@ -2525,126 +2525,126 @@
       <c r="H9" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36" t="s">
+      <c r="I9" s="43"/>
+      <c r="J9" s="43" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="36"/>
+      <c r="K9" s="43"/>
       <c r="L9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="77" t="s">
+      <c r="M9" s="105" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="44"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="94" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="103"/>
+      <c r="B10" s="104"/>
+      <c r="C10" s="104"/>
+      <c r="D10" s="104"/>
+      <c r="E10" s="104"/>
+      <c r="F10" s="104"/>
+      <c r="G10" s="78" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="94" t="s">
+      <c r="H10" s="78" t="s">
         <v>114</v>
       </c>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40" t="s">
+      <c r="I10" s="104"/>
+      <c r="J10" s="104"/>
+      <c r="K10" s="104"/>
+      <c r="L10" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="M10" s="78"/>
-    </row>
-    <row r="11" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="45"/>
-      <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="37"/>
-      <c r="K11" s="37"/>
-      <c r="L11" s="37"/>
-      <c r="M11" s="79"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="43" t="s">
+      <c r="M10" s="106"/>
+    </row>
+    <row r="11" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="99"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="80"/>
+      <c r="H11" s="80"/>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="44"/>
+      <c r="M11" s="107"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="98" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="36" t="s">
+      <c r="C12" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="36" t="s">
+      <c r="D12" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="36" t="s">
+      <c r="F12" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="94" t="s">
+      <c r="G12" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="H12" s="94" t="s">
+      <c r="H12" s="78" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36" t="s">
+      <c r="I12" s="43"/>
+      <c r="J12" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="K12" s="36"/>
-      <c r="L12" s="36" t="s">
+      <c r="K12" s="43"/>
+      <c r="L12" s="43" t="s">
         <v>86</v>
       </c>
       <c r="M12" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="40"/>
-      <c r="L13" s="40"/>
+    <row r="13" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="103"/>
+      <c r="B13" s="104"/>
+      <c r="C13" s="104"/>
+      <c r="D13" s="104"/>
+      <c r="E13" s="104"/>
+      <c r="F13" s="104"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="79"/>
+      <c r="I13" s="104"/>
+      <c r="J13" s="104"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="104"/>
       <c r="M13" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="45"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="96"/>
-      <c r="H14" s="96"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="37"/>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
+    <row r="14" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="99"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="80"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="44"/>
+      <c r="J14" s="44"/>
+      <c r="K14" s="44"/>
+      <c r="L14" s="44"/>
       <c r="M14" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
         <v>8</v>
       </c>
@@ -2683,44 +2683,6 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G10:G11"/>
     <mergeCell ref="M9:M11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="A12:A14"/>
@@ -2737,6 +2699,44 @@
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B0E7B62A-066D-41B6-B74D-35280CC4CFFE}"/>
@@ -2751,112 +2751,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE5EBCD-3AC3-4409-A2EA-4D4158C2CA26}">
   <dimension ref="A1:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="9" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="28.42578125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="9" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.44140625" style="9" customWidth="1"/>
+    <col min="8" max="8" width="28.44140625" style="9" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="9" customWidth="1"/>
+    <col min="10" max="10" width="34.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="9" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="9" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="9"/>
+    <col min="13" max="13" width="46.33203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="86" t="str">
+      <c r="B2" s="87" t="str">
         <f>'Listado Objetos Dominio'!A6</f>
         <v>Turno</v>
       </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-      <c r="F2" s="86"/>
-      <c r="G2" s="86"/>
-      <c r="H2" s="86"/>
-      <c r="I2" s="86"/>
-      <c r="J2" s="86"/>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
+      <c r="L2" s="87"/>
+      <c r="M2" s="88"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="88" t="str">
+      <c r="B3" s="89" t="str">
         <f>'Listado Objetos Dominio'!B6</f>
         <v>Objeto de dominio que representa uno de los turnos que representan un bloque de tiempo que el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="88"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="88"/>
-      <c r="H3" s="88"/>
-      <c r="I3" s="88"/>
-      <c r="J3" s="88"/>
-      <c r="K3" s="88"/>
-      <c r="L3" s="88"/>
-      <c r="M3" s="89"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
+      <c r="I3" s="89"/>
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="90"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="81"/>
+      <c r="C4" s="91"/>
       <c r="D4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="82" t="s">
+      <c r="E4" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="82"/>
-      <c r="G4" s="90" t="s">
+      <c r="F4" s="92"/>
+      <c r="G4" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="90"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="16" t="s">
         <v>26</v>
       </c>
@@ -2866,52 +2866,52 @@
       <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="91" t="s">
+      <c r="L4" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="92" t="s">
+      <c r="M4" s="95" t="s">
         <v>30</v>
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="93" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="81" t="s">
+      <c r="B5" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="81" t="s">
+      <c r="C5" s="91" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="70" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="82" t="s">
+      <c r="E5" s="92" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="82"/>
-      <c r="G5" s="83" t="s">
+      <c r="F5" s="92"/>
+      <c r="G5" s="100" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="84" t="s">
+      <c r="H5" s="100"/>
+      <c r="I5" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="85" t="s">
+      <c r="J5" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="80" t="s">
+      <c r="K5" s="97" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="91"/>
-      <c r="M5" s="92"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="93"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="49"/>
+      <c r="L5" s="94"/>
+      <c r="M5" s="95"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="96"/>
+      <c r="B6" s="91"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
@@ -2924,149 +2924,149 @@
       <c r="H6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="84"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="80"/>
-      <c r="L6" s="91"/>
-      <c r="M6" s="92"/>
-    </row>
-    <row r="7" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
+      <c r="I6" s="101"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="97"/>
+      <c r="L6" s="94"/>
+      <c r="M6" s="95"/>
+    </row>
+    <row r="7" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="86" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="94" t="s">
+      <c r="G7" s="78" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="94" t="s">
+      <c r="H7" s="78" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="35"/>
-      <c r="J7" s="35" t="s">
+      <c r="I7" s="86"/>
+      <c r="J7" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35" t="s">
+      <c r="K7" s="86"/>
+      <c r="L7" s="86" t="s">
         <v>96</v>
       </c>
       <c r="M7" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="35"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="95"/>
-      <c r="H8" s="95"/>
-      <c r="I8" s="35"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="86"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="79"/>
+      <c r="H8" s="79"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="86" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35"/>
-    </row>
-    <row r="10" spans="1:14" ht="108" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
+    <row r="9" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="86"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+    </row>
+    <row r="10" spans="1:14" ht="108" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="86" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="86" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="86" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="86" t="s">
         <v>92</v>
       </c>
       <c r="G10" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="94" t="s">
+      <c r="H10" s="78" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="35"/>
-      <c r="J10" s="35" t="s">
+      <c r="I10" s="86"/>
+      <c r="J10" s="86" t="s">
         <v>102</v>
       </c>
-      <c r="K10" s="94"/>
-      <c r="L10" s="35" t="s">
+      <c r="K10" s="78"/>
+      <c r="L10" s="86" t="s">
         <v>95</v>
       </c>
-      <c r="M10" s="35" t="s">
+      <c r="M10" s="86" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="35"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="86"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
       <c r="G11" s="109"/>
-      <c r="H11" s="95"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="95"/>
-      <c r="L11" s="35"/>
-      <c r="M11" s="35"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="35"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
+      <c r="H11" s="79"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="79"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="86"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="86"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
       <c r="G12" s="110"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="96"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-    </row>
-    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="H12" s="80"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+    </row>
+    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
         <v>8</v>
       </c>
@@ -3103,106 +3103,85 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="94" t="s">
+    <row r="14" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="94" t="s">
+      <c r="B14" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="94" t="s">
+      <c r="C14" s="78" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="94" t="s">
+      <c r="D14" s="78" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="94" t="s">
+      <c r="E14" s="78" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="94" t="s">
+      <c r="F14" s="78" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="94" t="s">
+      <c r="G14" s="78" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="94" t="s">
+      <c r="H14" s="78" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="94"/>
-      <c r="J14" s="36" t="s">
+      <c r="I14" s="78"/>
+      <c r="J14" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94" t="s">
+      <c r="K14" s="78"/>
+      <c r="L14" s="78" t="s">
         <v>95</v>
       </c>
-      <c r="M14" s="106" t="s">
+      <c r="M14" s="31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="96"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="96"/>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="96"/>
-      <c r="H15" s="96"/>
-      <c r="I15" s="96"/>
-      <c r="J15" s="37"/>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="107" t="s">
+    <row r="15" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="80"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="80"/>
+      <c r="D15" s="80"/>
+      <c r="E15" s="80"/>
+      <c r="F15" s="80"/>
+      <c r="G15" s="80"/>
+      <c r="H15" s="80"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="80"/>
+      <c r="L15" s="80"/>
+      <c r="M15" s="32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
       <c r="H21" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="M10:M12"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
     <mergeCell ref="F10:F12"/>
     <mergeCell ref="I10:I12"/>
     <mergeCell ref="J10:J12"/>
@@ -3219,16 +3198,37 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
     <mergeCell ref="K10:K12"/>
     <mergeCell ref="L10:L12"/>
-    <mergeCell ref="M10:M12"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="M8:M9"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{29F5E9C1-A6C7-4E2F-9918-9910FA7ACF50}"/>

</xml_diff>

<commit_message>
Terminando responsabilidades del enriquesido para el contexto agendas
</commit_message>
<xml_diff>
--- a/Doo-Doc/Nueva Version Victus/Event Storming/Agendas - Event Storming.xlsx
+++ b/Doo-Doc/Nueva Version Victus/Event Storming/Agendas - Event Storming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josez\Documents\Universidad IngeSistemas\Diseño Orientado a Objetos(DOO)\VictusProyect\victus-doc\Doo-Doc\Nueva Version Victus\Event Storming\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB47941C-CABF-4999-9E83-FC3FDABD2089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937B6849-1F68-4AB0-BCE8-27B6B846A47B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{FFDB2CDE-A71C-41B2-9368-C2C506410E3B}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="1" activeTab="3" xr2:uid="{FFDB2CDE-A71C-41B2-9368-C2C506410E3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="1" r:id="rId1"/>
@@ -1026,143 +1026,176 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1176,12 +1209,6 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1197,35 +1224,8 @@
     <xf numFmtId="0" fontId="5" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1641,7 +1641,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1652,19 +1652,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA54A37-9234-4843-BCF9-75FA1FE96664}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1674,7 +1674,7 @@
       <c r="C1" s="36"/>
       <c r="D1" s="37"/>
     </row>
-    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1684,7 +1684,7 @@
       <c r="C2" s="39"/>
       <c r="D2" s="40"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1698,7 +1698,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>Agendas</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>9</v>
       </c>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="D5" s="34"/>
     </row>
-    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -1760,108 +1760,108 @@
       <selection activeCell="F15" sqref="F15:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="9" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="29.88671875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="9" customWidth="1"/>
     <col min="8" max="8" width="31" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="37.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="9" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="9"/>
+    <col min="13" max="13" width="46.28515625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="55" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="47"/>
-      <c r="L2" s="47"/>
-      <c r="M2" s="48"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="49" t="str">
+      <c r="B3" s="58" t="str">
         <f>'Listado Objetos Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada una de las zonas comúnes que tendrán una agenda y respectivos turnos.</v>
       </c>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
-      <c r="K3" s="50"/>
-      <c r="L3" s="50"/>
-      <c r="M3" s="51"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="52" t="s">
+      <c r="B4" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="53"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="56" t="s">
+      <c r="F4" s="64"/>
+      <c r="G4" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="57"/>
+      <c r="H4" s="66"/>
       <c r="I4" s="16" t="s">
         <v>26</v>
       </c>
@@ -1871,52 +1871,52 @@
       <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="58" t="s">
+      <c r="L4" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="61" t="s">
+      <c r="M4" s="70" t="s">
         <v>30</v>
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="64" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="75" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="66" t="s">
+      <c r="C5" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="72" t="s">
+      <c r="F5" s="64"/>
+      <c r="G5" s="81" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="73"/>
-      <c r="I5" s="74" t="s">
+      <c r="H5" s="82"/>
+      <c r="I5" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="76" t="s">
+      <c r="J5" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="68" t="s">
+      <c r="K5" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="59"/>
-      <c r="M5" s="62"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="65"/>
-      <c r="B6" s="67"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="71"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="71"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="74"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
@@ -1929,29 +1929,29 @@
       <c r="H6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="75"/>
-      <c r="J6" s="77"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="63"/>
-    </row>
-    <row r="7" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="81" t="s">
+      <c r="I6" s="84"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="78"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="72"/>
+    </row>
+    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="78" t="s">
+      <c r="B7" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="78" t="s">
+      <c r="D7" s="43" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="78" t="s">
+      <c r="E7" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="78" t="s">
+      <c r="F7" s="43" t="s">
         <v>42</v>
       </c>
       <c r="G7" s="21" t="s">
@@ -1960,272 +1960,245 @@
       <c r="H7" s="27" t="s">
         <v>105</v>
       </c>
-      <c r="I7" s="78"/>
-      <c r="J7" s="78" t="s">
+      <c r="I7" s="43"/>
+      <c r="J7" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="K7" s="78"/>
-      <c r="L7" s="78" t="s">
+      <c r="K7" s="43"/>
+      <c r="L7" s="43" t="s">
         <v>46</v>
       </c>
       <c r="M7" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="82"/>
-      <c r="B8" s="79"/>
-      <c r="C8" s="79"/>
-      <c r="D8" s="79"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="78" t="s">
+    <row r="8" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="78" t="s">
+      <c r="H8" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="I8" s="79"/>
-      <c r="J8" s="79"/>
-      <c r="K8" s="79"/>
-      <c r="L8" s="79"/>
-      <c r="M8" s="41" t="s">
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="M8" s="85" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="82"/>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79"/>
-      <c r="I9" s="79"/>
-      <c r="J9" s="79"/>
-      <c r="K9" s="79"/>
-      <c r="L9" s="79"/>
-      <c r="M9" s="42"/>
-    </row>
-    <row r="10" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="83"/>
-      <c r="B10" s="80"/>
-      <c r="C10" s="80"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="80"/>
-      <c r="F10" s="80"/>
-      <c r="G10" s="80"/>
-      <c r="H10" s="80"/>
-      <c r="I10" s="80"/>
-      <c r="J10" s="80"/>
-      <c r="K10" s="80"/>
-      <c r="L10" s="80"/>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="51"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="51"/>
+      <c r="H9" s="51"/>
+      <c r="I9" s="51"/>
+      <c r="J9" s="51"/>
+      <c r="K9" s="51"/>
+      <c r="L9" s="51"/>
+      <c r="M9" s="86"/>
+    </row>
+    <row r="10" spans="1:14" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="50"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="44"/>
       <c r="M10" s="29" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="41" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="D11" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="43" t="s">
+      <c r="E11" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="H11" s="43" t="s">
+      <c r="H11" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43" t="s">
+      <c r="I11" s="41"/>
+      <c r="J11" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43" t="s">
+      <c r="K11" s="41"/>
+      <c r="L11" s="41" t="s">
         <v>45</v>
       </c>
       <c r="M11" s="28" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="44"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="44"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="42"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="42"/>
+      <c r="H12" s="42"/>
+      <c r="I12" s="42"/>
+      <c r="J12" s="42"/>
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
       <c r="M12" s="30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A13" s="84" t="s">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="43" t="s">
+      <c r="D13" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="43" t="s">
+      <c r="F13" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="78" t="s">
+      <c r="G13" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="78" t="s">
+      <c r="H13" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43" t="s">
+      <c r="I13" s="41"/>
+      <c r="J13" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="K13" s="43"/>
-      <c r="L13" s="43" t="s">
+      <c r="K13" s="41"/>
+      <c r="L13" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="M13" s="43" t="s">
+      <c r="M13" s="41" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="85"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
-      <c r="M14" s="44"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A15" s="86" t="s">
+    <row r="14" spans="1:14" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="47"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="42"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="86" t="s">
+      <c r="C15" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="86" t="s">
+      <c r="D15" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="86" t="s">
+      <c r="E15" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="86" t="s">
+      <c r="F15" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="G15" s="78" t="s">
+      <c r="G15" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="H15" s="78" t="s">
+      <c r="H15" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="I15" s="86"/>
-      <c r="J15" s="86" t="s">
+      <c r="I15" s="45"/>
+      <c r="J15" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="K15" s="86"/>
-      <c r="L15" s="86" t="s">
+      <c r="K15" s="45"/>
+      <c r="L15" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="M15" s="86" t="s">
+      <c r="M15" s="45" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="86"/>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="80"/>
-      <c r="H16" s="80"/>
-      <c r="I16" s="86"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="86"/>
-      <c r="L16" s="86"/>
-      <c r="M16" s="86"/>
+    <row r="16" spans="1:14" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="45"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="45"/>
+      <c r="K16" s="45"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="J13:J14"/>
-    <mergeCell ref="K13:K14"/>
-    <mergeCell ref="L13:L14"/>
-    <mergeCell ref="M13:M14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="G8:G10"/>
-    <mergeCell ref="H8:H10"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2242,18 +2215,45 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:I6"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="G8:G10"/>
+    <mergeCell ref="H8:H10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="J13:J14"/>
+    <mergeCell ref="K13:K14"/>
+    <mergeCell ref="L13:L14"/>
+    <mergeCell ref="M13:M14"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
+    <mergeCell ref="M15:M16"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="H15:H16"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{887014DF-6A3A-42A6-91E6-4E5CFF547499}"/>
@@ -2267,112 +2267,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D6BA9DD-BD15-4DCD-887C-675FC668E26D}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="9" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="9" customWidth="1"/>
     <col min="8" max="8" width="28" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="9" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="9"/>
+    <col min="13" max="13" width="46.28515625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="87" t="str">
+      <c r="B2" s="98" t="str">
         <f>'Listado Objetos Dominio'!A5</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="88"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="99"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="89" t="str">
+      <c r="B3" s="100" t="str">
         <f>'Listado Objetos Dominio'!B5</f>
         <v>Objeto de dominio que representaa cada una de las agendas que dónde el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="90"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="101"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="91"/>
+      <c r="C4" s="94"/>
       <c r="D4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="93" t="s">
+      <c r="F4" s="95"/>
+      <c r="G4" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="93"/>
+      <c r="H4" s="102"/>
       <c r="I4" s="16" t="s">
         <v>26</v>
       </c>
@@ -2382,52 +2382,52 @@
       <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="94" t="s">
+      <c r="L4" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="95" t="s">
+      <c r="M4" s="104" t="s">
         <v>30</v>
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="96" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="92"/>
-      <c r="G5" s="100" t="s">
+      <c r="F5" s="95"/>
+      <c r="G5" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="100"/>
-      <c r="I5" s="101" t="s">
+      <c r="H5" s="96"/>
+      <c r="I5" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="94"/>
-      <c r="M5" s="95"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="96"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="71"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="104"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="105"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
@@ -2440,83 +2440,83 @@
       <c r="H6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="95"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="98" t="s">
+      <c r="I6" s="97"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="104"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="43" t="s">
+      <c r="D7" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="41" t="s">
         <v>70</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="H7" s="43" t="s">
+      <c r="H7" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43" t="s">
+      <c r="I7" s="41"/>
+      <c r="J7" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43" t="s">
+      <c r="K7" s="41"/>
+      <c r="L7" s="41" t="s">
         <v>74</v>
       </c>
       <c r="M7" s="25" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="112.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="44"/>
+    <row r="8" spans="1:14" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="93"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9" s="98" t="s">
+    <row r="9" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="91" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="41" t="s">
         <v>75</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="F9" s="43" t="s">
+      <c r="F9" s="41" t="s">
         <v>71</v>
       </c>
       <c r="G9" s="21" t="s">
@@ -2525,126 +2525,126 @@
       <c r="H9" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43" t="s">
+      <c r="I9" s="41"/>
+      <c r="J9" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="K9" s="43"/>
+      <c r="K9" s="41"/>
       <c r="L9" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="M9" s="105" t="s">
+      <c r="M9" s="87" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="103"/>
-      <c r="B10" s="104"/>
-      <c r="C10" s="104"/>
-      <c r="D10" s="104"/>
-      <c r="E10" s="104"/>
-      <c r="F10" s="104"/>
-      <c r="G10" s="78" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="92"/>
+      <c r="B10" s="90"/>
+      <c r="C10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="90"/>
+      <c r="F10" s="90"/>
+      <c r="G10" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="I10" s="104"/>
-      <c r="J10" s="104"/>
-      <c r="K10" s="104"/>
-      <c r="L10" s="104" t="s">
+      <c r="I10" s="90"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="90"/>
+      <c r="L10" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="M10" s="106"/>
-    </row>
-    <row r="11" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="44"/>
-      <c r="F11" s="44"/>
-      <c r="G11" s="80"/>
-      <c r="H11" s="80"/>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="44"/>
-      <c r="M11" s="107"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="98" t="s">
+      <c r="M10" s="88"/>
+    </row>
+    <row r="11" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="93"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="44"/>
+      <c r="H11" s="44"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
+      <c r="K11" s="42"/>
+      <c r="L11" s="42"/>
+      <c r="M11" s="89"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="91" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="D12" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="F12" s="43" t="s">
+      <c r="F12" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="G12" s="78" t="s">
+      <c r="G12" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="H12" s="78" t="s">
+      <c r="H12" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43" t="s">
+      <c r="I12" s="41"/>
+      <c r="J12" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43" t="s">
+      <c r="K12" s="41"/>
+      <c r="L12" s="41" t="s">
         <v>86</v>
       </c>
       <c r="M12" s="23" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="103"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="104"/>
-      <c r="E13" s="104"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="79"/>
-      <c r="H13" s="79"/>
-      <c r="I13" s="104"/>
-      <c r="J13" s="104"/>
-      <c r="K13" s="104"/>
-      <c r="L13" s="104"/>
+    <row r="13" spans="1:14" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="92"/>
+      <c r="B13" s="90"/>
+      <c r="C13" s="90"/>
+      <c r="D13" s="90"/>
+      <c r="E13" s="90"/>
+      <c r="F13" s="90"/>
+      <c r="G13" s="51"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="90"/>
+      <c r="J13" s="90"/>
+      <c r="K13" s="90"/>
+      <c r="L13" s="90"/>
       <c r="M13" s="23" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="99"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="80"/>
-      <c r="H14" s="80"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="44"/>
+    <row r="14" spans="1:14" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="93"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
       <c r="M14" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
         <v>8</v>
       </c>
@@ -2683,6 +2683,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="M9:M11"/>
     <mergeCell ref="L10:L11"/>
     <mergeCell ref="A12:A14"/>
@@ -2699,44 +2737,6 @@
     <mergeCell ref="L12:L14"/>
     <mergeCell ref="J9:J11"/>
     <mergeCell ref="K9:K11"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{B0E7B62A-066D-41B6-B74D-35280CC4CFFE}"/>
@@ -2752,111 +2752,111 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B12"/>
+      <selection activeCell="C14" sqref="C14:C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="9" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="9" customWidth="1"/>
-    <col min="8" max="8" width="28.44140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="9" customWidth="1"/>
-    <col min="10" max="10" width="34.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="9" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="9" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="28.42578125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="9" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="9" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="9"/>
+    <col min="13" max="13" width="46.28515625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45"/>
-      <c r="M1" s="45"/>
-      <c r="N1" s="45"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="87" t="str">
+      <c r="B2" s="98" t="str">
         <f>'Listado Objetos Dominio'!A6</f>
         <v>Turno</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-      <c r="L2" s="87"/>
-      <c r="M2" s="88"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="99"/>
       <c r="N2" s="11"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="89" t="str">
+      <c r="B3" s="100" t="str">
         <f>'Listado Objetos Dominio'!B6</f>
         <v>Objeto de dominio que representa uno de los turnos que representan un bloque de tiempo que el residente podrá reservar.</v>
       </c>
-      <c r="C3" s="89"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
-      <c r="H3" s="89"/>
-      <c r="I3" s="89"/>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="90"/>
+      <c r="C3" s="100"/>
+      <c r="D3" s="100"/>
+      <c r="E3" s="100"/>
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="100"/>
+      <c r="I3" s="100"/>
+      <c r="J3" s="100"/>
+      <c r="K3" s="100"/>
+      <c r="L3" s="100"/>
+      <c r="M3" s="101"/>
       <c r="N3" s="13"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="91"/>
+      <c r="C4" s="94"/>
       <c r="D4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="92" t="s">
+      <c r="E4" s="95" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="92"/>
-      <c r="G4" s="93" t="s">
+      <c r="F4" s="95"/>
+      <c r="G4" s="102" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="93"/>
+      <c r="H4" s="102"/>
       <c r="I4" s="16" t="s">
         <v>26</v>
       </c>
@@ -2866,52 +2866,52 @@
       <c r="K4" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="L4" s="94" t="s">
+      <c r="L4" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="M4" s="95" t="s">
+      <c r="M4" s="104" t="s">
         <v>30</v>
       </c>
       <c r="N4" s="13"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="96" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="91" t="s">
+      <c r="C5" s="94" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="70" t="s">
+      <c r="D5" s="79" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="92" t="s">
+      <c r="E5" s="95" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="92"/>
-      <c r="G5" s="100" t="s">
+      <c r="F5" s="95"/>
+      <c r="G5" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="H5" s="100"/>
-      <c r="I5" s="101" t="s">
+      <c r="H5" s="96"/>
+      <c r="I5" s="97" t="s">
         <v>35</v>
       </c>
-      <c r="J5" s="102" t="s">
+      <c r="J5" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="106" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="94"/>
-      <c r="M5" s="95"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="96"/>
-      <c r="B6" s="91"/>
-      <c r="C6" s="91"/>
-      <c r="D6" s="71"/>
+      <c r="L5" s="103"/>
+      <c r="M5" s="104"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="105"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="19" t="s">
         <v>38</v>
       </c>
@@ -2924,149 +2924,149 @@
       <c r="H6" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="101"/>
-      <c r="J6" s="102"/>
-      <c r="K6" s="97"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="95"/>
-    </row>
-    <row r="7" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="86" t="s">
+      <c r="I6" s="97"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="103"/>
+      <c r="M6" s="104"/>
+    </row>
+    <row r="7" spans="1:14" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="B7" s="86" t="s">
+      <c r="B7" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="C7" s="86" t="s">
+      <c r="C7" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="86" t="s">
+      <c r="D7" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="86" t="s">
+      <c r="E7" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="F7" s="86" t="s">
+      <c r="F7" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="78" t="s">
+      <c r="G7" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="H7" s="78" t="s">
+      <c r="H7" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="I7" s="86"/>
-      <c r="J7" s="86" t="s">
+      <c r="I7" s="45"/>
+      <c r="J7" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="K7" s="86"/>
-      <c r="L7" s="86" t="s">
+      <c r="K7" s="45"/>
+      <c r="L7" s="45" t="s">
         <v>96</v>
       </c>
       <c r="M7" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="86"/>
-      <c r="B8" s="86"/>
-      <c r="C8" s="86"/>
-      <c r="D8" s="86"/>
-      <c r="E8" s="86"/>
-      <c r="F8" s="86"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="86"/>
-      <c r="J8" s="86"/>
-      <c r="K8" s="86"/>
-      <c r="L8" s="86"/>
-      <c r="M8" s="86" t="s">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
+      <c r="M8" s="45" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="86"/>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="80"/>
-      <c r="H9" s="80"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-    </row>
-    <row r="10" spans="1:14" ht="108" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="86" t="s">
+    <row r="9" spans="1:14" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="45"/>
+      <c r="J9" s="45"/>
+      <c r="K9" s="45"/>
+      <c r="L9" s="45"/>
+      <c r="M9" s="45"/>
+    </row>
+    <row r="10" spans="1:14" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="86" t="s">
+      <c r="B10" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="86" t="s">
+      <c r="C10" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="86" t="s">
+      <c r="E10" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="86" t="s">
+      <c r="F10" s="45" t="s">
         <v>92</v>
       </c>
       <c r="G10" s="108" t="s">
         <v>93</v>
       </c>
-      <c r="H10" s="78" t="s">
+      <c r="H10" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86" t="s">
+      <c r="I10" s="45"/>
+      <c r="J10" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="K10" s="78"/>
-      <c r="L10" s="86" t="s">
+      <c r="K10" s="43"/>
+      <c r="L10" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="M10" s="86" t="s">
+      <c r="M10" s="45" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="86"/>
-      <c r="B11" s="86"/>
-      <c r="C11" s="86"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="86"/>
-      <c r="F11" s="86"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="109"/>
-      <c r="H11" s="79"/>
-      <c r="I11" s="86"/>
-      <c r="J11" s="86"/>
-      <c r="K11" s="79"/>
-      <c r="L11" s="86"/>
-      <c r="M11" s="86"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="86"/>
-      <c r="B12" s="86"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="86"/>
-      <c r="E12" s="86"/>
-      <c r="F12" s="86"/>
+      <c r="H11" s="51"/>
+      <c r="I11" s="45"/>
+      <c r="J11" s="45"/>
+      <c r="K11" s="51"/>
+      <c r="L11" s="45"/>
+      <c r="M11" s="45"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
+      <c r="D12" s="45"/>
+      <c r="E12" s="45"/>
+      <c r="F12" s="45"/>
       <c r="G12" s="110"/>
-      <c r="H12" s="80"/>
-      <c r="I12" s="86"/>
-      <c r="J12" s="86"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="86"/>
-      <c r="M12" s="86"/>
-    </row>
-    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="45"/>
+      <c r="K12" s="44"/>
+      <c r="L12" s="45"/>
+      <c r="M12" s="45"/>
+    </row>
+    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
         <v>8</v>
       </c>
@@ -3103,88 +3103,103 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="78" t="s">
+    <row r="14" spans="1:14" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="78" t="s">
+      <c r="B14" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="78" t="s">
+      <c r="C14" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="78" t="s">
+      <c r="D14" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="78" t="s">
+      <c r="E14" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="78" t="s">
+      <c r="F14" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="78" t="s">
+      <c r="G14" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="H14" s="78" t="s">
+      <c r="H14" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="I14" s="78"/>
-      <c r="J14" s="43" t="s">
+      <c r="I14" s="43"/>
+      <c r="J14" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="K14" s="78"/>
-      <c r="L14" s="78" t="s">
+      <c r="K14" s="43"/>
+      <c r="L14" s="43" t="s">
         <v>95</v>
       </c>
       <c r="M14" s="31" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
-      <c r="B15" s="80"/>
-      <c r="C15" s="80"/>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80"/>
-      <c r="H15" s="80"/>
-      <c r="I15" s="80"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="80"/>
-      <c r="L15" s="80"/>
+    <row r="15" spans="1:14" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="44"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
       <c r="M15" s="32" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" s="26"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H18" s="26"/>
     </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H19" s="26"/>
     </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H20" s="26"/>
     </row>
-    <row r="21" spans="8:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H21" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="M10:M12"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="I10:I12"/>
-    <mergeCell ref="J10:J12"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="K10:K12"/>
+    <mergeCell ref="L10:L12"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="B7:B9"/>
@@ -3201,34 +3216,19 @@
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="M10:M12"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="I10:I12"/>
+    <mergeCell ref="J10:J12"/>
     <mergeCell ref="G7:G9"/>
     <mergeCell ref="H7:H9"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="K10:K12"/>
-    <mergeCell ref="L10:L12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{29F5E9C1-A6C7-4E2F-9918-9910FA7ACF50}"/>

</xml_diff>